<commit_message>
Revert "Merge branch 'PWMTesting_2_Lawrence' of https://github.com/Agile-and-Adaptive-Robotics/Muscle_Sensory into PWMTesting_2_Lawrence"
This reverts commit af80296e510cfab2e62d151d5f14bbf5597082b6, reversing
changes made to ba956a58db6c06af00cd21b725bdbe5ae0ac15a8.
</commit_message>
<xml_diff>
--- a/DataCollection/2022Jan27_LoadCalibration.xlsx
+++ b/DataCollection/2022Jan27_LoadCalibration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Intel\Documents\GitHub\Muscle_Sensory\DataCollection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lawre\Documents\GitHub\Muscle-Sensory\DataCollection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CEE3B5-E20E-40B3-B1EE-8891B8AB4348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861AFFBA-EC90-46B1-9D50-C08845BB515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{78597D30-0546-4EF1-87D6-6F5522700415}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{78597D30-0546-4EF1-87D6-6F5522700415}"/>
   </bookViews>
   <sheets>
     <sheet name="10mm" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -75,6 +77,9 @@
     <t>Gain = 1046</t>
   </si>
   <si>
+    <t>Resistor 47Ohm</t>
+  </si>
+  <si>
     <t>Arduino Output(Min)</t>
   </si>
   <si>
@@ -94,9 +99,6 @@
   </si>
   <si>
     <t>Resistor 470 Ohm</t>
-  </si>
-  <si>
-    <t>Resistor 47 Ohm</t>
   </si>
 </sst>
 </file>
@@ -7945,37 +7947,37 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -7983,21 +7985,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -8005,10 +8007,10 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>7</v>
@@ -8023,7 +8025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>0</v>
       </c>
@@ -8047,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -8071,7 +8073,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -8095,7 +8097,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>15</v>
       </c>
@@ -8119,7 +8121,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>20</v>
       </c>
@@ -8143,7 +8145,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>25</v>
       </c>
@@ -8167,7 +8169,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>30</v>
       </c>
@@ -8191,7 +8193,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>35</v>
       </c>
@@ -8215,7 +8217,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>37.5</v>
       </c>
@@ -8239,7 +8241,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>40</v>
       </c>
@@ -8264,7 +8266,7 @@
         <v>1.2552000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="E19" s="5">
         <f t="shared" si="2"/>
@@ -8285,33 +8287,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A219C13-4757-44D3-88EB-70D463DA07F4}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="32.21875" customWidth="1"/>
+    <col min="7" max="7" width="22.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8319,21 +8321,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8341,10 +8343,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -8359,7 +8361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -8380,7 +8382,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -8401,7 +8403,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>10</v>
       </c>
@@ -8422,7 +8424,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>15</v>
       </c>
@@ -8443,7 +8445,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -8464,7 +8466,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>25</v>
       </c>
@@ -8485,7 +8487,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -8506,7 +8508,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>35</v>
       </c>
@@ -8527,7 +8529,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>37.5</v>
       </c>
@@ -8548,10 +8550,10 @@
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
       <c r="N16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>40</v>
       </c>
@@ -8576,7 +8578,7 @@
         <v>0.53400000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="E18" s="5">
         <f t="shared" si="1"/>
@@ -8597,32 +8599,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{057DF3D1-51D5-431A-9AE6-9FF188C12E35}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="109.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8630,21 +8631,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8652,10 +8653,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>7</v>
@@ -8670,7 +8671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -8690,7 +8691,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="7"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
@@ -8710,7 +8711,7 @@
       <c r="G9" s="8"/>
       <c r="H9" s="7"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>10</v>
       </c>
@@ -8730,7 +8731,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>15</v>
       </c>
@@ -8750,7 +8751,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>20</v>
       </c>
@@ -8770,7 +8771,7 @@
       <c r="G12" s="8"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>25</v>
       </c>
@@ -8790,7 +8791,7 @@
       <c r="G13" s="8"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>30</v>
       </c>
@@ -8810,7 +8811,7 @@
       <c r="G14" s="8"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>35</v>
       </c>
@@ -8830,7 +8831,7 @@
       <c r="G15" s="8"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>37.5</v>
       </c>
@@ -8850,7 +8851,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>40</v>
       </c>
@@ -8869,7 +8870,7 @@
       </c>
       <c r="H17" s="12"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11"/>
       <c r="E18" s="5"/>
       <c r="H18" s="12"/>

</xml_diff>